<commit_message>
v2 and proxying note updates
</commit_message>
<xml_diff>
--- a/cuak_versions.xlsx
+++ b/cuak_versions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cleanup\l2_cuak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58301727-FD69-4311-BFC7-765D01809A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444366D3-8C34-488E-AFC0-592D8F15848E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -36,10 +36,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>cuak_v1</t>
-  </si>
-  <si>
-    <t>The first containerized Chrome deployment</t>
+    <t>cuak_v1-1.95</t>
+  </si>
+  <si>
+    <t>The first containerized Chrome deployments (Multi-VM behind ALB, VNC session routing issue)</t>
+  </si>
+  <si>
+    <t>cuak_v2</t>
+  </si>
+  <si>
+    <t>FIRST STABLE RELEASE (Implements Redis Caching to find VM running Chrome container)</t>
   </si>
 </sst>
 </file>
@@ -358,16 +364,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -392,6 +398,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>45738</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>